<commit_message>
rt rw as string
</commit_message>
<xml_diff>
--- a/Input/XLSGM1218/HPDB - XLSGM1218.xlsx
+++ b/Input/XLSGM1218/HPDB - XLSGM1218.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\MBKM\force\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\MBKM\force\Input\XLSGM1218\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BD3368-252E-4194-AA4B-0854FA55198D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D63645-7FA2-449C-9B54-A5DBCBF59609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="44" r:id="rId6"/>
+    <pivotCache cacheId="4" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5863" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5863" uniqueCount="466">
   <si>
     <t>ACQUISITION_CLASS</t>
   </si>
@@ -1439,6 +1439,9 @@
   </si>
   <si>
     <t>BIZ</t>
+  </si>
+  <si>
+    <t>002</t>
   </si>
 </sst>
 </file>
@@ -1479,7 +1482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1487,8 +1490,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1507,7 +1511,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="rian raffi" refreshedDate="45370.481041550927" createdVersion="5" refreshedVersion="8" minRefreshableVersion="3" recordCount="92" xr:uid="{00C6AABB-D6E1-4FC6-BA0E-1DB16A8056FE}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="rian raffi" refreshedDate="45372.388738657406" createdVersion="5" refreshedVersion="8" minRefreshableVersion="3" recordCount="92" xr:uid="{00C6AABB-D6E1-4FC6-BA0E-1DB16A8056FE}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:AX93" sheet="HPDB_Excel"/>
   </cacheSource>
@@ -1612,7 +1616,7 @@
       <sharedItems/>
     </cacheField>
     <cacheField name="FAT_LATITUDE" numFmtId="0">
-      <sharedItems/>
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="-5219555" maxValue="-5219555"/>
     </cacheField>
     <cacheField name="BUILDING_LATITUDE" numFmtId="0">
       <sharedItems/>
@@ -1852,7 +1856,7 @@
     <s v="119.438824"/>
     <s v="-5.217626"/>
     <s v="119.445176"/>
-    <s v="-5.219916"/>
+    <n v="-5219555"/>
     <s v="-5.219991"/>
     <s v="119.445168"/>
     <s v="-"/>
@@ -6554,7 +6558,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="HPDB_Excel" cacheId="44" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" missingCaption="" updatedVersion="8" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" indent="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="HPDB_Excel" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" missingCaption="" updatedVersion="8" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" indent="0">
   <location ref="A1:B94" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="50">
     <pivotField name="ACQUISITION_CLASS" defaultSubtotal="0"/>
@@ -7310,7 +7314,7 @@
       <c r="A2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7318,7 +7322,7 @@
       <c r="A3" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7326,7 +7330,7 @@
       <c r="A4" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7334,7 +7338,7 @@
       <c r="A5" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7342,7 +7346,7 @@
       <c r="A6" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7350,7 +7354,7 @@
       <c r="A7" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7358,7 +7362,7 @@
       <c r="A8" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7366,7 +7370,7 @@
       <c r="A9" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7374,7 +7378,7 @@
       <c r="A10" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7382,7 +7386,7 @@
       <c r="A11" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7390,7 +7394,7 @@
       <c r="A12" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7398,7 +7402,7 @@
       <c r="A13" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7406,7 +7410,7 @@
       <c r="A14" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7414,7 +7418,7 @@
       <c r="A15" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7422,7 +7426,7 @@
       <c r="A16" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7430,7 +7434,7 @@
       <c r="A17" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7438,7 +7442,7 @@
       <c r="A18" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7446,7 +7450,7 @@
       <c r="A19" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7454,7 +7458,7 @@
       <c r="A20" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7462,7 +7466,7 @@
       <c r="A21" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7470,7 +7474,7 @@
       <c r="A22" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7478,7 +7482,7 @@
       <c r="A23" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7486,7 +7490,7 @@
       <c r="A24" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7494,7 +7498,7 @@
       <c r="A25" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7502,7 +7506,7 @@
       <c r="A26" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7510,7 +7514,7 @@
       <c r="A27" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7518,7 +7522,7 @@
       <c r="A28" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7526,7 +7530,7 @@
       <c r="A29" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7534,7 +7538,7 @@
       <c r="A30" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7542,7 +7546,7 @@
       <c r="A31" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7550,7 +7554,7 @@
       <c r="A32" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7558,7 +7562,7 @@
       <c r="A33" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B33" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7566,7 +7570,7 @@
       <c r="A34" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B34" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7574,7 +7578,7 @@
       <c r="A35" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7582,7 +7586,7 @@
       <c r="A36" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B36" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7590,7 +7594,7 @@
       <c r="A37" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7598,7 +7602,7 @@
       <c r="A38" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7606,7 +7610,7 @@
       <c r="A39" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="B39" s="5">
+      <c r="B39" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7614,7 +7618,7 @@
       <c r="A40" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="B40" s="5">
+      <c r="B40" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7622,7 +7626,7 @@
       <c r="A41" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="B41" s="5">
+      <c r="B41" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7630,7 +7634,7 @@
       <c r="A42" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B42" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7638,7 +7642,7 @@
       <c r="A43" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="B43" s="5">
+      <c r="B43" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7646,7 +7650,7 @@
       <c r="A44" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="B44" s="5">
+      <c r="B44" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7654,7 +7658,7 @@
       <c r="A45" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="B45" s="5">
+      <c r="B45" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7662,7 +7666,7 @@
       <c r="A46" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="B46" s="5">
+      <c r="B46" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7670,7 +7674,7 @@
       <c r="A47" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="B47" s="5">
+      <c r="B47" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7678,7 +7682,7 @@
       <c r="A48" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="B48" s="5">
+      <c r="B48" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7686,7 +7690,7 @@
       <c r="A49" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="B49" s="5">
+      <c r="B49" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7694,7 +7698,7 @@
       <c r="A50" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="B50" s="5">
+      <c r="B50" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7702,7 +7706,7 @@
       <c r="A51" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="B51" s="5">
+      <c r="B51" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7710,7 +7714,7 @@
       <c r="A52" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="B52" s="5">
+      <c r="B52" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7718,7 +7722,7 @@
       <c r="A53" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="B53" s="5">
+      <c r="B53" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7726,7 +7730,7 @@
       <c r="A54" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="B54" s="5">
+      <c r="B54" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7734,7 +7738,7 @@
       <c r="A55" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="B55" s="5">
+      <c r="B55" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7742,7 +7746,7 @@
       <c r="A56" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="B56" s="5">
+      <c r="B56" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7750,7 +7754,7 @@
       <c r="A57" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="B57" s="5">
+      <c r="B57" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7758,7 +7762,7 @@
       <c r="A58" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="B58" s="5">
+      <c r="B58" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7766,7 +7770,7 @@
       <c r="A59" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="B59" s="5">
+      <c r="B59" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7774,7 +7778,7 @@
       <c r="A60" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="B60" s="5">
+      <c r="B60" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7782,7 +7786,7 @@
       <c r="A61" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="B61" s="5">
+      <c r="B61" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7790,7 +7794,7 @@
       <c r="A62" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="B62" s="5">
+      <c r="B62" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7798,7 +7802,7 @@
       <c r="A63" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="B63" s="5">
+      <c r="B63" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7806,7 +7810,7 @@
       <c r="A64" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="B64" s="5">
+      <c r="B64" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7814,7 +7818,7 @@
       <c r="A65" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="B65" s="5">
+      <c r="B65" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7822,7 +7826,7 @@
       <c r="A66" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="B66" s="5">
+      <c r="B66" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7830,7 +7834,7 @@
       <c r="A67" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="B67" s="5">
+      <c r="B67" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7838,7 +7842,7 @@
       <c r="A68" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="B68" s="5">
+      <c r="B68" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7846,7 +7850,7 @@
       <c r="A69" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="B69" s="5">
+      <c r="B69" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7854,7 +7858,7 @@
       <c r="A70" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="B70" s="5">
+      <c r="B70" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7862,7 +7866,7 @@
       <c r="A71" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="B71" s="5">
+      <c r="B71" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7870,7 +7874,7 @@
       <c r="A72" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="B72" s="5">
+      <c r="B72" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7878,7 +7882,7 @@
       <c r="A73" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="B73" s="5">
+      <c r="B73" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7886,7 +7890,7 @@
       <c r="A74" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="B74" s="5">
+      <c r="B74" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7894,7 +7898,7 @@
       <c r="A75" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="B75" s="5">
+      <c r="B75" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7902,7 +7906,7 @@
       <c r="A76" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="B76" s="5">
+      <c r="B76" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7910,7 +7914,7 @@
       <c r="A77" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="B77" s="5">
+      <c r="B77" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7918,7 +7922,7 @@
       <c r="A78" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="B78" s="5">
+      <c r="B78" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7926,7 +7930,7 @@
       <c r="A79" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="B79" s="5">
+      <c r="B79" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7934,7 +7938,7 @@
       <c r="A80" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="B80" s="5">
+      <c r="B80" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7942,7 +7946,7 @@
       <c r="A81" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="B81" s="5">
+      <c r="B81" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7950,7 +7954,7 @@
       <c r="A82" s="4" t="s">
         <v>415</v>
       </c>
-      <c r="B82" s="5">
+      <c r="B82" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7958,7 +7962,7 @@
       <c r="A83" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="B83" s="5">
+      <c r="B83" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7966,7 +7970,7 @@
       <c r="A84" s="4" t="s">
         <v>423</v>
       </c>
-      <c r="B84" s="5">
+      <c r="B84" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7974,7 +7978,7 @@
       <c r="A85" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="B85" s="5">
+      <c r="B85" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7982,7 +7986,7 @@
       <c r="A86" s="4" t="s">
         <v>431</v>
       </c>
-      <c r="B86" s="5">
+      <c r="B86" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7990,7 +7994,7 @@
       <c r="A87" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="B87" s="5">
+      <c r="B87" s="6">
         <v>1</v>
       </c>
     </row>
@@ -7998,7 +8002,7 @@
       <c r="A88" s="4" t="s">
         <v>437</v>
       </c>
-      <c r="B88" s="5">
+      <c r="B88" s="6">
         <v>1</v>
       </c>
     </row>
@@ -8006,7 +8010,7 @@
       <c r="A89" s="4" t="s">
         <v>441</v>
       </c>
-      <c r="B89" s="5">
+      <c r="B89" s="6">
         <v>1</v>
       </c>
     </row>
@@ -8014,7 +8018,7 @@
       <c r="A90" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="B90" s="5">
+      <c r="B90" s="6">
         <v>1</v>
       </c>
     </row>
@@ -8022,7 +8026,7 @@
       <c r="A91" s="4" t="s">
         <v>449</v>
       </c>
-      <c r="B91" s="5">
+      <c r="B91" s="6">
         <v>1</v>
       </c>
     </row>
@@ -8030,7 +8034,7 @@
       <c r="A92" s="4" t="s">
         <v>453</v>
       </c>
-      <c r="B92" s="5">
+      <c r="B92" s="6">
         <v>1</v>
       </c>
     </row>
@@ -8038,7 +8042,7 @@
       <c r="A93" s="4" t="s">
         <v>457</v>
       </c>
-      <c r="B93" s="5">
+      <c r="B93" s="6">
         <v>1</v>
       </c>
     </row>
@@ -8046,7 +8050,7 @@
       <c r="A94" s="4" t="s">
         <v>462</v>
       </c>
-      <c r="B94" s="5">
+      <c r="B94" s="6">
         <v>92</v>
       </c>
     </row>
@@ -8061,8 +8065,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AX93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AH3" sqref="AH3"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8481,7 +8485,7 @@
       <c r="AG3" t="s">
         <v>75</v>
       </c>
-      <c r="AH3" s="6">
+      <c r="AH3" s="5">
         <v>-5219555</v>
       </c>
       <c r="AI3" t="s">
@@ -9351,8 +9355,8 @@
       <c r="S9" t="s">
         <v>51</v>
       </c>
-      <c r="T9" t="s">
-        <v>64</v>
+      <c r="T9" s="7" t="s">
+        <v>465</v>
       </c>
       <c r="U9" t="s">
         <v>65</v>

</xml_diff>